<commit_message>
Wrote code so board cells and players are drawn - pair programming
</commit_message>
<xml_diff>
--- a/data/boardLayoutUpdate.xlsx
+++ b/data/boardLayoutUpdate.xlsx
@@ -3,18 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\CSCI306New\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9600"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19110" windowHeight="11580"/>
   </bookViews>
   <sheets>
     <sheet name="boardLayoutUpdate" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -135,7 +131,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -208,6 +204,30 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -221,7 +241,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -239,6 +259,10 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -247,8 +271,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF33CC"/>
       <color rgb="FF00FFFF"/>
-      <color rgb="FFFF33CC"/>
     </mruColors>
   </colors>
   <extLst>
@@ -528,7 +552,7 @@
   <dimension ref="A1:Z34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Z6" sqref="Z6"/>
+      <selection activeCell="N29" sqref="N29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -574,7 +598,7 @@
       <c r="F1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="15" t="s">
         <v>1</v>
       </c>
       <c r="H1" s="3" t="s">
@@ -610,7 +634,7 @@
       <c r="R1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="S1" s="16" t="s">
         <v>1</v>
       </c>
       <c r="T1" s="2" t="s">
@@ -1356,7 +1380,7 @@
       </c>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="12" t="s">
         <v>1</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -1668,7 +1692,7 @@
       <c r="X14" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="Y14" s="3" t="s">
+      <c r="Y14" s="13" t="s">
         <v>1</v>
       </c>
       <c r="Z14" s="1">
@@ -2417,7 +2441,7 @@
       <c r="G24" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="H24" s="3" t="s">
+      <c r="H24" s="18" t="s">
         <v>1</v>
       </c>
       <c r="I24" s="3" t="s">
@@ -2447,7 +2471,7 @@
       <c r="Q24" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="R24" s="3" t="s">
+      <c r="R24" s="17" t="s">
         <v>1</v>
       </c>
       <c r="S24" s="11" t="s">

</xml_diff>